<commit_message>
Add approx size to table 1
</commit_message>
<xml_diff>
--- a/Data/Table1.xlsx
+++ b/Data/Table1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://outlookuga-my.sharepoint.com/personal/ccz99536_uga_edu/Documents/Cruises/NES_CCS_Comparison/AcidotropicManuscript/AcidotropicDyes/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{234F9DD3-26B4-B74E-B3E1-077CA923C6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5270C12D-EBB9-7F4F-8784-5541EA38FEEA}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{234F9DD3-26B4-B74E-B3E1-077CA923C6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF43C56C-283A-EB4E-846A-5DFD001690A7}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="1440" windowWidth="28040" windowHeight="17440" xr2:uid="{C714B500-95DA-1A49-BF0B-C97DEF21A789}"/>
+    <workbookView xWindow="30400" yWindow="-1300" windowWidth="38080" windowHeight="20780" xr2:uid="{C714B500-95DA-1A49-BF0B-C97DEF21A789}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="72">
   <si>
     <t>Culture</t>
   </si>
@@ -401,6 +401,54 @@
   </si>
   <si>
     <t>Mixotroph?&lt;sup&gt;2&lt;/sup&gt;</t>
+  </si>
+  <si>
+    <t>10 to 85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 to 100 </t>
+  </si>
+  <si>
+    <t>5 to 22</t>
+  </si>
+  <si>
+    <t>6 to 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 to 6 </t>
+  </si>
+  <si>
+    <t>10 to 14</t>
+  </si>
+  <si>
+    <t>12 to 14</t>
+  </si>
+  <si>
+    <t>35 to 130</t>
+  </si>
+  <si>
+    <t>18 to 26</t>
+  </si>
+  <si>
+    <t>2 to 4</t>
+  </si>
+  <si>
+    <t>6 to 8</t>
+  </si>
+  <si>
+    <t>15 to 55</t>
+  </si>
+  <si>
+    <t>4 to 15</t>
+  </si>
+  <si>
+    <t>8 to 12</t>
+  </si>
+  <si>
+    <t>3 to 5</t>
+  </si>
+  <si>
+    <t>Approximate size range (µm)</t>
   </si>
 </sst>
 </file>
@@ -463,12 +511,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,6 +534,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -803,10 +857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB75994B-6D02-B24F-94A2-B1587318A1B8}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -814,7 +868,7 @@
     <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -839,8 +893,11 @@
       <c r="H1" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -865,8 +922,11 @@
       <c r="H2" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -891,8 +951,11 @@
       <c r="H3" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -917,8 +980,11 @@
       <c r="H4" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -943,8 +1009,11 @@
       <c r="H5" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -969,8 +1038,11 @@
       <c r="H6" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -995,8 +1067,11 @@
       <c r="H7" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1021,8 +1096,11 @@
       <c r="H8" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -1047,8 +1125,11 @@
       <c r="H9" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -1073,8 +1154,11 @@
       <c r="H10" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -1099,8 +1183,11 @@
       <c r="H11" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -1125,8 +1212,11 @@
       <c r="H12" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -1151,8 +1241,11 @@
       <c r="H13" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -1177,8 +1270,11 @@
       <c r="H14" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -1203,8 +1299,11 @@
       <c r="H15" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -1229,8 +1328,11 @@
       <c r="H16" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -1255,8 +1357,11 @@
       <c r="H17" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
@@ -1281,8 +1386,11 @@
       <c r="H18" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>43</v>
       </c>
@@ -1306,6 +1414,9 @@
       </c>
       <c r="H19" s="2" t="s">
         <v>52</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
micromonas picoeuk specific gate update
</commit_message>
<xml_diff>
--- a/Data/Table1.xlsx
+++ b/Data/Table1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://outlookuga-my.sharepoint.com/personal/ccz99536_uga_edu/Documents/Cruises/NES_CCS_Comparison/AcidotropicManuscript/AcidotropicDyes/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{234F9DD3-26B4-B74E-B3E1-077CA923C6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF43C56C-283A-EB4E-846A-5DFD001690A7}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{234F9DD3-26B4-B74E-B3E1-077CA923C6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D72BB4D-0EFF-2845-ADA1-C6397E7A5478}"/>
   <bookViews>
     <workbookView xWindow="30400" yWindow="-1300" windowWidth="38080" windowHeight="20780" xr2:uid="{C714B500-95DA-1A49-BF0B-C97DEF21A789}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="73">
   <si>
     <t>Culture</t>
   </si>
@@ -397,9 +397,6 @@
     <t>North Atlantic</t>
   </si>
   <si>
-    <t>Mixotroph&lt;sup&gt;3&lt;/sup&gt;</t>
-  </si>
-  <si>
     <t>Mixotroph?&lt;sup&gt;2&lt;/sup&gt;</t>
   </si>
   <si>
@@ -449,6 +446,12 @@
   </si>
   <si>
     <t>Approximate size range (µm)</t>
+  </si>
+  <si>
+    <t>Phototroph?</t>
+  </si>
+  <si>
+    <t>Mixotroph&lt;sup&gt;4&lt;/sup&gt;</t>
   </si>
 </sst>
 </file>
@@ -860,7 +863,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -894,7 +897,7 @@
         <v>47</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -923,7 +926,7 @@
         <v>45</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -952,7 +955,7 @@
         <v>45</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -981,7 +984,7 @@
         <v>45</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1010,7 +1013,7 @@
         <v>45</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1039,7 +1042,7 @@
         <v>46</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1068,7 +1071,7 @@
         <v>48</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1097,7 +1100,7 @@
         <v>48</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1117,7 +1120,7 @@
         <v>110</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>12</v>
@@ -1126,7 +1129,7 @@
         <v>49</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1155,7 +1158,7 @@
         <v>49</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1184,7 +1187,7 @@
         <v>48</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1213,7 +1216,7 @@
         <v>46</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1233,7 +1236,7 @@
         <v>70</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>26</v>
@@ -1242,7 +1245,7 @@
         <v>46</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1271,7 +1274,7 @@
         <v>50</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1300,7 +1303,7 @@
         <v>45</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1329,7 +1332,7 @@
         <v>45</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -1358,7 +1361,7 @@
         <v>51</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1387,7 +1390,7 @@
         <v>51</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1407,7 +1410,7 @@
         <v>70</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>26</v>
@@ -1416,7 +1419,7 @@
         <v>52</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change table size range to cytpix values
</commit_message>
<xml_diff>
--- a/Data/Table1.xlsx
+++ b/Data/Table1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://outlookuga-my.sharepoint.com/personal/ccz99536_uga_edu/Documents/Cruises/NES_CCS_Comparison/AcidotropicManuscript/AcidotropicDyes/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{234F9DD3-26B4-B74E-B3E1-077CA923C6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D72BB4D-0EFF-2845-ADA1-C6397E7A5478}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="8_{234F9DD3-26B4-B74E-B3E1-077CA923C6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{851E7FDC-95E4-434F-B6F1-4D2494170A19}"/>
   <bookViews>
-    <workbookView xWindow="30400" yWindow="-1300" windowWidth="38080" windowHeight="20780" xr2:uid="{C714B500-95DA-1A49-BF0B-C97DEF21A789}"/>
+    <workbookView xWindow="29500" yWindow="2720" windowWidth="38080" windowHeight="20780" xr2:uid="{C714B500-95DA-1A49-BF0B-C97DEF21A789}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="76">
   <si>
     <t>Culture</t>
   </si>
@@ -400,58 +400,67 @@
     <t>Mixotroph?&lt;sup&gt;2&lt;/sup&gt;</t>
   </si>
   <si>
-    <t>10 to 85</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 to 100 </t>
-  </si>
-  <si>
-    <t>5 to 22</t>
-  </si>
-  <si>
-    <t>6 to 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 to 6 </t>
-  </si>
-  <si>
-    <t>10 to 14</t>
-  </si>
-  <si>
-    <t>12 to 14</t>
-  </si>
-  <si>
-    <t>35 to 130</t>
-  </si>
-  <si>
-    <t>18 to 26</t>
-  </si>
-  <si>
-    <t>2 to 4</t>
-  </si>
-  <si>
     <t>6 to 8</t>
   </si>
   <si>
-    <t>15 to 55</t>
-  </si>
-  <si>
-    <t>4 to 15</t>
-  </si>
-  <si>
-    <t>8 to 12</t>
-  </si>
-  <si>
-    <t>3 to 5</t>
-  </si>
-  <si>
-    <t>Approximate size range (µm)</t>
-  </si>
-  <si>
     <t>Phototroph?</t>
   </si>
   <si>
     <t>Mixotroph&lt;sup&gt;4&lt;/sup&gt;</t>
+  </si>
+  <si>
+    <t>6 to 9</t>
+  </si>
+  <si>
+    <t>5 to 10</t>
+  </si>
+  <si>
+    <t>7 to 31</t>
+  </si>
+  <si>
+    <t>12 to 15</t>
+  </si>
+  <si>
+    <t>10 to 17</t>
+  </si>
+  <si>
+    <t>7 to 13</t>
+  </si>
+  <si>
+    <t>16 to &gt;72</t>
+  </si>
+  <si>
+    <t>17 to &gt;72</t>
+  </si>
+  <si>
+    <t>14 to 37</t>
+  </si>
+  <si>
+    <t>8 to 14</t>
+  </si>
+  <si>
+    <t>13 to &gt;72</t>
+  </si>
+  <si>
+    <t>8 to 10</t>
+  </si>
+  <si>
+    <t>6 to 7</t>
+  </si>
+  <si>
+    <t>8 to 15</t>
+  </si>
+  <si>
+    <t>9 to 17</t>
+  </si>
+  <si>
+    <t>4 to 20</t>
+  </si>
+  <si>
+    <t>CytPixSize</t>
+  </si>
+  <si>
+    <t>1 to 3&lt;sup&gt;8&lt;/sup&gt;</t>
   </si>
 </sst>
 </file>
@@ -514,14 +523,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -863,7 +870,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -897,7 +904,7 @@
         <v>47</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -925,8 +932,8 @@
       <c r="H2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>55</v>
+      <c r="I2" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -954,8 +961,8 @@
       <c r="H3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>55</v>
+      <c r="I3" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -983,8 +990,8 @@
       <c r="H4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>55</v>
+      <c r="I4" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1012,8 +1019,8 @@
       <c r="H5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>56</v>
+      <c r="I5" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1041,8 +1048,8 @@
       <c r="H6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>57</v>
+      <c r="I6" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1070,8 +1077,8 @@
       <c r="H7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>58</v>
+      <c r="I7" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1099,8 +1106,8 @@
       <c r="H8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>59</v>
+      <c r="I8" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1128,8 +1135,8 @@
       <c r="H9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I9" s="5" t="s">
-        <v>60</v>
+      <c r="I9" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1157,8 +1164,8 @@
       <c r="H10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>61</v>
+      <c r="I10" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1186,8 +1193,8 @@
       <c r="H11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>62</v>
+      <c r="I11" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1215,8 +1222,8 @@
       <c r="H12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I12" s="5" t="s">
-        <v>63</v>
+      <c r="I12" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1236,7 +1243,7 @@
         <v>70</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>26</v>
@@ -1244,8 +1251,8 @@
       <c r="H13" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I13" s="5" t="s">
-        <v>64</v>
+      <c r="I13" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1273,8 +1280,8 @@
       <c r="H14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>65</v>
+      <c r="I14" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1302,8 +1309,8 @@
       <c r="H15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>66</v>
+      <c r="I15" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1331,8 +1338,8 @@
       <c r="H16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>67</v>
+      <c r="I16" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -1360,8 +1367,8 @@
       <c r="H17" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>68</v>
+      <c r="I17" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1389,8 +1396,8 @@
       <c r="H18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>69</v>
+      <c r="I18" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1410,7 +1417,7 @@
         <v>70</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>26</v>
@@ -1418,8 +1425,8 @@
       <c r="H19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I19" s="6" t="s">
-        <v>68</v>
+      <c r="I19" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update 72 µm to 74 µm
</commit_message>
<xml_diff>
--- a/Data/Table1.xlsx
+++ b/Data/Table1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://outlookuga-my.sharepoint.com/personal/ccz99536_uga_edu/Documents/Cruises/NES_CCS_Comparison/AcidotropicManuscript/AcidotropicDyes/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="8_{234F9DD3-26B4-B74E-B3E1-077CA923C6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{851E7FDC-95E4-434F-B6F1-4D2494170A19}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{234F9DD3-26B4-B74E-B3E1-077CA923C6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D35F6F26-07CA-F045-9730-C494FD701C2C}"/>
   <bookViews>
-    <workbookView xWindow="29500" yWindow="2720" windowWidth="38080" windowHeight="20780" xr2:uid="{C714B500-95DA-1A49-BF0B-C97DEF21A789}"/>
+    <workbookView xWindow="30240" yWindow="-1140" windowWidth="38080" windowHeight="20780" xr2:uid="{C714B500-95DA-1A49-BF0B-C97DEF21A789}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -427,12 +427,6 @@
     <t>7 to 13</t>
   </si>
   <si>
-    <t>16 to &gt;72</t>
-  </si>
-  <si>
-    <t>17 to &gt;72</t>
-  </si>
-  <si>
     <t>14 to 37</t>
   </si>
   <si>
@@ -461,6 +455,12 @@
   </si>
   <si>
     <t>1 to 3&lt;sup&gt;8&lt;/sup&gt;</t>
+  </si>
+  <si>
+    <t>16 to &gt;74</t>
+  </si>
+  <si>
+    <t>17 to &gt;74</t>
   </si>
 </sst>
 </file>
@@ -870,7 +870,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -904,7 +904,7 @@
         <v>47</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -962,7 +962,7 @@
         <v>45</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -991,7 +991,7 @@
         <v>45</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1020,7 +1020,7 @@
         <v>45</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1049,7 +1049,7 @@
         <v>46</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1078,7 +1078,7 @@
         <v>48</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1107,7 +1107,7 @@
         <v>48</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1136,7 +1136,7 @@
         <v>49</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1165,7 +1165,7 @@
         <v>49</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1194,7 +1194,7 @@
         <v>48</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1223,7 +1223,7 @@
         <v>46</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1252,7 +1252,7 @@
         <v>46</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>